<commit_message>
Build 1 complete, works fine in IDE. needs some work elsewhere
</commit_message>
<xml_diff>
--- a/backgrounds/Bonds.xlsx
+++ b/backgrounds/Bonds.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="306">
   <si>
     <t>Acolyte</t>
   </si>
@@ -25,15 +25,9 @@
     <t>Athlete</t>
   </si>
   <si>
-    <t>Azorius Functionary</t>
-  </si>
-  <si>
     <t>Black Fist Double Agent</t>
   </si>
   <si>
-    <t>Boros Legionnaire</t>
-  </si>
-  <si>
     <t>Caravan Specialist</t>
   </si>
   <si>
@@ -61,9 +55,6 @@
     <t>Criminal</t>
   </si>
   <si>
-    <t>Dragon Casualty</t>
-  </si>
-  <si>
     <t>Earthspur Miner</t>
   </si>
   <si>
@@ -88,12 +79,6 @@
     <t>Gate Urchin</t>
   </si>
   <si>
-    <t>Golgari Agent</t>
-  </si>
-  <si>
-    <t>Gruul Anarch</t>
-  </si>
-  <si>
     <t>Gambler</t>
   </si>
   <si>
@@ -118,9 +103,6 @@
     <t>Hillsfar Smuggler</t>
   </si>
   <si>
-    <t>House Agent</t>
-  </si>
-  <si>
     <t>Inheritor</t>
   </si>
   <si>
@@ -133,9 +115,6 @@
     <t>Iron Route Bandit</t>
   </si>
   <si>
-    <t>Izzet Engineer</t>
-  </si>
-  <si>
     <t>Knight</t>
   </si>
   <si>
@@ -148,9 +127,6 @@
     <t>Noble</t>
   </si>
   <si>
-    <t>Orzhov Representative</t>
-  </si>
-  <si>
     <t>Outlander</t>
   </si>
   <si>
@@ -166,9 +142,6 @@
     <t>Plaintiff</t>
   </si>
   <si>
-    <t>Rakdos Cultist</t>
-  </si>
-  <si>
     <t>Rival Intern</t>
   </si>
   <si>
@@ -181,18 +154,12 @@
     <t>Secret Identity</t>
   </si>
   <si>
-    <t>Selesnya Initiate</t>
-  </si>
-  <si>
     <t>Shade Fanatic</t>
   </si>
   <si>
     <t>Shipwright</t>
   </si>
   <si>
-    <t>Simic Scientist</t>
-  </si>
-  <si>
     <t>Smuggler</t>
   </si>
   <si>
@@ -220,9 +187,6 @@
     <t>I was framed for a crime I did not commit, and seek to bring the true culprit to justice.</t>
   </si>
   <si>
-    <t>I would lay down my life for Aurelia and the angels.</t>
-  </si>
-  <si>
     <t>My brother has a farm In Elmwood and I've helped him and his neigbors move their goods to Mulmaster and other surrounding towns. Those are good people.</t>
   </si>
   <si>
@@ -244,9 +208,6 @@
     <t>The elves took me in when I had nowhere else to go. In return, I do what I can to help elves in need.</t>
   </si>
   <si>
-    <t>I have sworn vengeance on the Maimed Virulence and those that follow him.</t>
-  </si>
-  <si>
     <t>The people of the Earthspur mines are my family. I will do anything to protect them.</t>
   </si>
   <si>
@@ -271,12 +232,6 @@
     <t>The Joydancers of Lliira gave me my instrument when I really needed food. I hate them for that.</t>
   </si>
   <si>
-    <t>I cherish the finger of a family member who was petrified by a medusa.</t>
-  </si>
-  <si>
-    <t>I am determined that one day I will lead my clan - or a new one.</t>
-  </si>
-  <si>
     <t>One person in particular owes me a lot of money, and I need to keep them alive if I want to be repaid.</t>
   </si>
   <si>
@@ -295,9 +250,6 @@
     <t>I am loyal to the Rogues Guild and would do anything for them.</t>
   </si>
   <si>
-    <t>My house is my family. I would do anything for it.</t>
-  </si>
-  <si>
     <t>One of my crop-mates is my dearest friend, and I hope we will face each other in the final trial.</t>
   </si>
   <si>
@@ -307,9 +259,6 @@
     <t>I cannot leave a harmed animal behind; I must save it or put it out of its misery.</t>
   </si>
   <si>
-    <t>I have dedicated my life to finding a solution to a scientific problem.</t>
-  </si>
-  <si>
     <t>I will face any challenge to win the approval of my family.</t>
   </si>
   <si>
@@ -319,9 +268,6 @@
     <t>I will face any challenge to win the approval of my family,</t>
   </si>
   <si>
-    <t>The unbearable weight of my debt has driven me to desperation.</t>
-  </si>
-  <si>
     <t>My family, clan, or tribe is the most important thing in my life, even when they are far from me.</t>
   </si>
   <si>
@@ -337,27 +283,18 @@
     <t>Others hurt in the same accident that hurt me are my new family. I'll make sure they're taken care of.</t>
   </si>
   <si>
-    <t>I have belonged to the same performance troupe for years, and these people mean everything to me.</t>
-  </si>
-  <si>
     <t>I have a family member in need. I consider them in everything I do.</t>
   </si>
   <si>
     <t>The humans of Hillsfar have inflicted terrible harm on me, my family, and my race. I will have revenge.</t>
   </si>
   <si>
-    <t>I would give my life in the defense of the small enclave where I first encountered Mat'Selesnya.</t>
-  </si>
-  <si>
     <t>They say the Shade broke the bonds of mortality; I want to find out how.</t>
   </si>
   <si>
     <t>I must visit all the oceans of the world and behold the shops that sail there.</t>
   </si>
   <si>
-    <t>I helped create a krasis that I love like a pet and would carry with me everywhere … except it's the size of a building, and it might eat me.</t>
-  </si>
-  <si>
     <t>My vessel was stolen from me, and I burn with the desire to recover it.</t>
   </si>
   <si>
@@ -379,9 +316,6 @@
     <t>I am a part of an underground network that smuggles innocent civilians out of the city prior to being raided by the authorities.</t>
   </si>
   <si>
-    <t>I owe my life to the Boros captain who took me in when I was living on the streets.</t>
-  </si>
-  <si>
     <t>A caravan I lead was attacked by bandits and many innocents died. I swear that I will avenge them by killing any bandits I encounter.</t>
   </si>
   <si>
@@ -403,9 +337,6 @@
     <t>I seek revenge against the people of Hillsfar for driving my family into the forest.</t>
   </si>
   <si>
-    <t>I long to reunite with friends and family who may dwell among the Phlan Refugees, and protect them.</t>
-  </si>
-  <si>
     <t>A deep gnome saved my life when I was injured and alone. I owe his people a great debt.</t>
   </si>
   <si>
@@ -430,12 +361,6 @@
     <t>Busking has taught me to love music above all else.</t>
   </si>
   <si>
-    <t>I have an identical twin who is as different from me as any person could be.</t>
-  </si>
-  <si>
-    <t>I would give my life for my clan chieftain.</t>
-  </si>
-  <si>
     <t>I'm loyal to the friend or family member who taught me how to gamble.</t>
   </si>
   <si>
@@ -454,9 +379,6 @@
     <t>I love the city of Hillsfar and my fellow Hillsfarians, despite the recent problems.</t>
   </si>
   <si>
-    <t>I love someone from another house, but the relationship is forbidden.</t>
-  </si>
-  <si>
     <t>I am in love with a vizier.</t>
   </si>
   <si>
@@ -466,18 +388,12 @@
     <t>I leave behind my own personal calling cards when I do a job.</t>
   </si>
   <si>
-    <t>I'll never forget the laboratory where I learned my skills, or the other attendants who learned alongside me.</t>
-  </si>
-  <si>
     <t>My house's alliance with another noble family must be sustained at all costs.</t>
   </si>
   <si>
     <t>My family and I are loyal supporters of High Blade Jaseen Drakehorn. Our fortunes are inexorably tied to hers. I would do anything to support her.</t>
   </si>
   <si>
-    <t>I'm duty-bound to obey the dictates of an ancestor on the Ghost Council.</t>
-  </si>
-  <si>
     <t>An injury to the unspoiled wilderness of my home is an injury to me.</t>
   </si>
   <si>
@@ -493,27 +409,18 @@
     <t>The rulers of this place were kind to me, and they have my lifelong devotion.</t>
   </si>
   <si>
-    <t>A blood witch told me I have a special destiny to fulfill, and I'm trying to figure out what it is.</t>
-  </si>
-  <si>
     <t>My peers keep me grounded.</t>
   </si>
   <si>
     <t>I am part of an underground network that smuggles non-humans into and out of the city.</t>
   </si>
   <si>
-    <t>I love beasts and plants of all kinds, and am loath to harm them.</t>
-  </si>
-  <si>
     <t>The whispers in my head remind me that there is power to be found in the shadows.</t>
   </si>
   <si>
     <t>Much of the treasure I claim will be used to enrich my community.</t>
   </si>
   <si>
-    <t>In my laboratory, I discovered something that I think could eliminate half the life on Ravnica.</t>
-  </si>
-  <si>
     <t>I intend to become the leader of the network of smugglers that I belong to.</t>
   </si>
   <si>
@@ -535,9 +442,6 @@
     <t>I miss the glory days of Phlan, before the coming of the dragon.</t>
   </si>
   <si>
-    <t>My fellow legionnaires are my family.</t>
-  </si>
-  <si>
     <t>The Soldiery are mostly good guys who understand the importance of protecting the roads. The City Watch is who you have to look out for. If they are inspecting your goods, get ready to pay a fine.</t>
   </si>
   <si>
@@ -559,9 +463,6 @@
     <t>My family lost everything when they were driven from Hillsfar. I strive to rebuild that fortune.</t>
   </si>
   <si>
-    <t>While a prisoner of the Maimed Virulence, I overheard rumors of an item or treasure the Dragon seeks. I will have that treasure for myself!</t>
-  </si>
-  <si>
     <t>I must behold and preserve the natural beauty of places below the earth.</t>
   </si>
   <si>
@@ -586,12 +487,6 @@
     <t>The Rogues' Guild spared me when I did a job without cutting them in. I owe them a great debt.</t>
   </si>
   <si>
-    <t>I want to lead one faction of the guild to a new position of dominance.</t>
-  </si>
-  <si>
-    <t>The chieftain of another clan has a grudge against me.</t>
-  </si>
-  <si>
     <t>The person who saved me from my gambling addiction is the only reason I'm alive today.</t>
   </si>
   <si>
@@ -610,9 +505,6 @@
     <t>I admire the elves. I help them whenever I can.</t>
   </si>
   <si>
-    <t>Someone I love was killed by a rival faction within my house, and I wil l have revenge.</t>
-  </si>
-  <si>
     <t>I am particularly drawn to one of the five gods, and I want nothing more than to win that god’s particular favor.</t>
   </si>
   <si>
@@ -622,18 +514,12 @@
     <t>I do not trust people who do not have a pet, mount, or furry companion.</t>
   </si>
   <si>
-    <t>I'm convinced it was sabotage that destroyed my first laboratory and killed many of my friends, and I seek revenge against whoever did it.</t>
-  </si>
-  <si>
     <t>Nothing is more important than the other members of my family.</t>
   </si>
   <si>
     <t>Like many families who were close to High Blade Selfaril Uoumdolphin, mine has suffered greatly since his fall. We honor his memory in secret.</t>
   </si>
   <si>
-    <t>I value my worldly goods more highly than my mortal life.</t>
-  </si>
-  <si>
     <t>I will bring terrible wrath down on the evildoers who destroyed my homeland.</t>
   </si>
   <si>
@@ -649,27 +535,18 @@
     <t>My parents worry about me, but I'll make them proud.</t>
   </si>
   <si>
-    <t>I'm secretly hoping that I can change the cult from the inside, using my influence to help rein in the wanton violence.</t>
-  </si>
-  <si>
     <t>My past mistakes cost someone else dearly. I have to rectify that.</t>
   </si>
   <si>
     <t>I am a partisan. I commit minor acts of defiance against the First Lord and Red Plumes when I can.</t>
   </si>
   <si>
-    <t>A healer nursed me to recovery from a mortal illness.</t>
-  </si>
-  <si>
     <t>For the glory of Netheril, I will grow in power.</t>
   </si>
   <si>
     <t>I must find a kind of wood rumored to possess magical qualities.</t>
   </si>
   <si>
-    <t>The other researchers in my clade are my family - a big, eccentric family including members and parts of many species.</t>
-  </si>
-  <si>
     <t>I owe a debt that cannot be repaid in gold.</t>
   </si>
   <si>
@@ -691,9 +568,6 @@
     <t>I seek to prove myself worthy of joining the Black Fist as a member of their order.</t>
   </si>
   <si>
-    <t>I wield the same Boros weapon my grandparent did, for the honor of our family.</t>
-  </si>
-  <si>
     <t>The new commander of Southroad Tower, Capt. Holke, understands the importance of safe roads. He's hired me for several jobs and I'm grateful.</t>
   </si>
   <si>
@@ -715,9 +589,6 @@
     <t>The forest has provided me with food and shelter. In return, I protect forests and those who dwell within.</t>
   </si>
   <si>
-    <t>I seek to reclaim and rebuild my former life to the best of my ability.</t>
-  </si>
-  <si>
     <t>Gems hold a special fascination for me, more than gold, land, magic, or power.</t>
   </si>
   <si>
@@ -742,12 +613,6 @@
     <t>I know people hate the Red Plumes, but some of them were really good to me. I help Red Plumes whenever I can, and I respect them. They're just doing what they have to do to get by in this world.</t>
   </si>
   <si>
-    <t>I love spending time in the moss-covered building where I took part in my first reclamation mission.</t>
-  </si>
-  <si>
-    <t>I am devoted to a sacred site in the midst of the rubblebelt.</t>
-  </si>
-  <si>
     <t>A patron once fronted me money in exchange for a percentage of my winnings. I owe them a debt of gratitude. And a lot of cash.</t>
   </si>
   <si>
@@ -766,9 +631,6 @@
     <t>A gnome helped me once. I pay the favor forward.</t>
   </si>
   <si>
-    <t>I don't care about the house as a whole, but I would do anything for my old mentor.</t>
-  </si>
-  <si>
     <t>I am more devoted to Naktamun and its people than I am to any of the ideals of the gods.</t>
   </si>
   <si>
@@ -778,18 +640,12 @@
     <t>The pelt I wear on my back was from an animal that died saving my life. I will always cherish it.</t>
   </si>
   <si>
-    <t>I have the schematics for an invention that I hope to build one day, once I have the necessary resources.</t>
-  </si>
-  <si>
     <t>I am in love with the heir of a family that my family despises.</t>
   </si>
   <si>
     <t>My family plotted with Rassendyll Uoumdolphin brother usurped brother as High Blade. Betrayal is the quickest route to power.</t>
   </si>
   <si>
-    <t>An oligarch publicly humiliated me, and I will exact revenge on that whole family.</t>
-  </si>
-  <si>
     <t>I am the last of my tribe, and it is up to me to ensure their names enter legend.</t>
   </si>
   <si>
@@ -805,27 +661,18 @@
     <t>The only bond that matters is the one holding my money pouch to my belt.</t>
   </si>
   <si>
-    <t>I own something that Rakdos once touched (it's seared black at the spot), and I cherish it.</t>
-  </si>
-  <si>
     <t>A childhood mentor put me on my current path. If I succeed, I want to repay that mentor in some way.</t>
   </si>
   <si>
     <t>I am a spy. I report on events in and around Hillfar.</t>
   </si>
   <si>
-    <t>I'll sing the invitation of Mat'Selesnya with my dying breath.</t>
-  </si>
-  <si>
     <t>I once lived in Hillsfar, I was chased out before I was able to say farewell.</t>
   </si>
   <si>
     <t>I repair broken things to redeem what’s broken in myself.</t>
   </si>
   <si>
-    <t>The laboratory where I did my research contains everything that is precious to me.</t>
-  </si>
-  <si>
     <t>After one last job, I will retire from the business.</t>
   </si>
   <si>
@@ -847,9 +694,6 @@
     <t>My sister was killed by a Tear of Virulence, and now I feed them false information whenever possible.</t>
   </si>
   <si>
-    <t>I ran with the Rakdos in my youth, and I'm striving to atone for my past misdeeds.</t>
-  </si>
-  <si>
     <t>There's always a road I haven't traveled before. I'm always looking for new places to explore.</t>
   </si>
   <si>
@@ -871,9 +715,6 @@
     <t>I am deeply, tragically in love with someone whose racial lifespan is far longer or shorter than mine.</t>
   </si>
   <si>
-    <t>I have been reborn as a child of Vorgansharax. I will claim my birthright as his chosen heir and successor.</t>
-  </si>
-  <si>
     <t>I want to explore new depths and scale new heights.</t>
   </si>
   <si>
@@ -898,12 +739,6 @@
     <t>I will be wealthy some day. My descendants will live in comfort and style.</t>
   </si>
   <si>
-    <t>I found something in the sewer that must never come to light.</t>
-  </si>
-  <si>
-    <t>My weapon is made from the first raktusk I ever hunted.</t>
-  </si>
-  <si>
     <t>A criminal syndicate I once played for isn't happy I left the game, and its enforcers are looking for me.</t>
   </si>
   <si>
@@ -922,9 +757,6 @@
     <t>I enjoy tricking the Red Plumes at every opportunity.</t>
   </si>
   <si>
-    <t>My house must evolve, and I'll lead the evolution.</t>
-  </si>
-  <si>
     <t>My weapon was a gift from a beloved trainer who died in an accident.</t>
   </si>
   <si>
@@ -934,18 +766,12 @@
     <t>If my pet does not like you, I do not like you!</t>
   </si>
   <si>
-    <t>A fellow student and I are racing to solve the same scientific puzzle.</t>
-  </si>
-  <si>
     <t>My loyalty to my sovereign is unwavering.</t>
   </si>
   <si>
     <t>Wealth and power are nothing. Fulfillment can only be found in artistic expression.</t>
   </si>
   <si>
-    <t>My faith in the Obzedat never wavers.</t>
-  </si>
-  <si>
     <t>I suffer awful visions of a coming disaster and will do anything to prevent it.</t>
   </si>
   <si>
@@ -961,27 +787,18 @@
     <t>The other new hires at Acquisitions Incorporated are my allies. We have each other's backs.</t>
   </si>
   <si>
-    <t>I want to be better at my chosen form of performance than any other member of my troupe.</t>
-  </si>
-  <si>
     <t>I value an oath of loyalty I took to a group of friends over everything else in my life.</t>
   </si>
   <si>
     <t>My secret identity is the only thing protecting me from the Arena. I will stop at nothing to maintain it.</t>
   </si>
   <si>
-    <t>I cherish a leaf from Vitu-Ghazi that changes color with the seasons, even though it is no longer attached to the tree.</t>
-  </si>
-  <si>
     <t>My true love was a killed by the Red Plumes; I plot to make them suffer.</t>
   </si>
   <si>
     <t>I will craft a boat capable of sailing through the most dangerous of storms.</t>
   </si>
   <si>
-    <t>I will get revenge on the shortsighted fool who killed my precious krasis creation.</t>
-  </si>
-  <si>
     <t>I was tricked by a fellow smuggler who stole something precious from me. I will find that thief.</t>
   </si>
   <si>
@@ -1003,9 +820,6 @@
     <t>My family was wrongly imprisoned, and I act as an informant in order to secure their release.</t>
   </si>
   <si>
-    <t>I do what I can to help out the spouse of a comrade who died in battle.</t>
-  </si>
-  <si>
     <t>Wealth and power mean little without the freedom to go where and when you want.</t>
   </si>
   <si>
@@ -1027,9 +841,6 @@
     <t>Members of my extended family did not make it to the camps or have been kidnapped to fight in the Arena. I search for them tirelessly.</t>
   </si>
   <si>
-    <t>I attribute my survival to the work of the divine, and seek to prove myself worthy of the honor.</t>
-  </si>
-  <si>
     <t>Someday I'm going to find the mother lode, then I'll spend the rest of my life in luxury.</t>
   </si>
   <si>
@@ -1054,12 +865,6 @@
     <t>I know how hard life on the streets is. I do everything I can for those who have less than me.</t>
   </si>
   <si>
-    <t>I am forever grateful to the reclaimer who found me floating facedown in the sewer, moments from death.</t>
-  </si>
-  <si>
-    <t>GrrrRRAAAAGGHH! [I will do anything to prove myself greater than my siblings or ancestors.]</t>
-  </si>
-  <si>
     <t>Urchins once helped me find marks for my games. Now I'm driven to help them escape the streets.</t>
   </si>
   <si>
@@ -1078,9 +883,6 @@
     <t>I smuggled agricultural goods for non-human farmers. I try to help them when I can.</t>
   </si>
   <si>
-    <t>I'm determined to impress the leaders of my house, and to become a leader myself.</t>
-  </si>
-  <si>
     <t>I carry a memento of my time as an acolyte, and I treasure it above all other things.</t>
   </si>
   <si>
@@ -1090,18 +892,12 @@
     <t>Once you’ve ridden with me and fought by my side, I’ll be there for you odds be damned.</t>
   </si>
   <si>
-    <t>I would do anything the guildmaster told me to do.</t>
-  </si>
-  <si>
     <t>The common folk must see me as a hero of the people.</t>
   </si>
   <si>
     <t>It's not how you feel, who you know, or what you can do - it's how you look, and I look fabulous.</t>
   </si>
   <si>
-    <t>I want to prove myself more worthy than an older sibling and thereby ensure that I inherit a greater share of my parents' wealth.</t>
-  </si>
-  <si>
     <t>It is my duty to provide children to sustain my tribe.</t>
   </si>
   <si>
@@ -1117,25 +913,16 @@
     <t>My legal counsel is my best friend. I owe all my forthcoming opportunities to their hard work.</t>
   </si>
   <si>
-    <t>I am devoted to Rakdos and live to impress him.</t>
-  </si>
-  <si>
     <t>Although I don’t get along well with people, my pet means the world to me.</t>
   </si>
   <si>
     <t>I am madly in love with a human who does not know my true identity, and I fear rejection if I reveal it.</t>
   </si>
   <si>
-    <t>Every member of the conclave is my kin, and I would fight for any one of them.</t>
-  </si>
-  <si>
     <t>I had a loved one die in the arena at Hillsfar; I am out to prove I am stronger than them!</t>
   </si>
   <si>
     <t>A kraken destroyed my masterpiece; its teeth shall adorn my hearth.</t>
-  </si>
-  <si>
-    <t>Everything I do is an attempt to impress someone I love.</t>
   </si>
   <si>
     <t>I give most of my profits to a charitable cause, and I don't like to brag about it.</t>
@@ -1433,10 +1220,10 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -1564,1203 +1351,972 @@
       </c>
       <c r="BA1" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="BG1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="BH1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="BI1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="BJ1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="BK1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="BL1" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="X2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AW2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="AK2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AY2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BA2" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="BA2" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="BC2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="BD2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="BE2" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="BF2" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="BG2" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="BH2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="BI2" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="BJ2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="BK2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="BL2" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z3" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF3" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="AH3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="AJ3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK3" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="AL3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="AN3" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="AO3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="AP3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="AQ3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="AR3" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="AS3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU3" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="AV3" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="AW3" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="AX3" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="AY3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA3" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AN3" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AO3" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AP3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AQ3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AR3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="AS3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AT3" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AU3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="AV3" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="AW3" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="AX3" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AY3" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AZ3" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="BA3" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="BB3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="BC3" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="BD3" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="BE3" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="BF3" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="BG3" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="BH3" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="BI3" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="BJ3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="BK3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="BL3" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AM4" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="AN4" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="AO4" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="AP4" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="AQ4" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="AR4" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="AS4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AT4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AU4" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="AV4" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="AW4" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="AX4" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="AY4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="BA4" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="AG4" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="AJ4" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="AO4" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AP4" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="AQ4" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AR4" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="AS4" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="AT4" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU4" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV4" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="AW4" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="AX4" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="AY4" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="AZ4" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="BA4" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="BB4" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="BC4" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="BD4" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="BE4" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="BF4" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="BG4" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="BH4" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="BI4" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="BJ4" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="BK4" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="BL4" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="AG5" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AH5" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="AK5" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="AP5" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="AR5" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AT5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="AU5" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="AV5" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AW5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AX5" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AY5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="BA5" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="AG5" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="AJ5" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="AK5" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="AL5" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="AM5" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="AN5" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="AO5" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="AP5" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AQ5" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="AR5" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="AS5" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="AT5" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="AU5" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="AV5" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="AW5" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="AX5" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="AY5" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="AZ5" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="BA5" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="BB5" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="BC5" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="BD5" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="BE5" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="BF5" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="BG5" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="BH5" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="BI5" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="BJ5" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="BK5" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="BL5" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>273</v>
+        <v>222</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>274</v>
+        <v>223</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>275</v>
+        <v>224</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>276</v>
+        <v>225</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>273</v>
+        <v>226</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>277</v>
+        <v>227</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>278</v>
+        <v>228</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>279</v>
+        <v>229</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>280</v>
+        <v>230</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>282</v>
+        <v>232</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>284</v>
+        <v>231</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>285</v>
+        <v>230</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>283</v>
+        <v>234</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>282</v>
+        <v>235</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>287</v>
+        <v>237</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>288</v>
+        <v>238</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>289</v>
+        <v>239</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>290</v>
+        <v>240</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>291</v>
+        <v>241</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>293</v>
+        <v>231</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>294</v>
+        <v>231</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>295</v>
+        <v>243</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>296</v>
+        <v>244</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>297</v>
+        <v>245</v>
       </c>
       <c r="AC6" s="2" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>298</v>
+        <v>240</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>299</v>
+        <v>248</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>300</v>
+        <v>249</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>301</v>
+        <v>250</v>
       </c>
       <c r="AI6" s="2" t="s">
-        <v>302</v>
+        <v>251</v>
       </c>
       <c r="AJ6" s="2" t="s">
-        <v>303</v>
+        <v>230</v>
       </c>
       <c r="AK6" s="2" t="s">
-        <v>293</v>
+        <v>252</v>
       </c>
       <c r="AL6" s="2" t="s">
-        <v>304</v>
+        <v>251</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>305</v>
+        <v>253</v>
       </c>
       <c r="AN6" s="2" t="s">
-        <v>306</v>
+        <v>254</v>
       </c>
       <c r="AO6" s="2" t="s">
-        <v>307</v>
+        <v>255</v>
       </c>
       <c r="AP6" s="2" t="s">
-        <v>308</v>
+        <v>256</v>
       </c>
       <c r="AQ6" s="2" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="AR6" s="2" t="s">
-        <v>309</v>
+        <v>258</v>
       </c>
       <c r="AS6" s="2" t="s">
-        <v>308</v>
+        <v>232</v>
       </c>
       <c r="AT6" s="2" t="s">
-        <v>310</v>
+        <v>254</v>
       </c>
       <c r="AU6" s="2" t="s">
-        <v>311</v>
+        <v>259</v>
       </c>
       <c r="AV6" s="2" t="s">
-        <v>312</v>
+        <v>260</v>
       </c>
       <c r="AW6" s="2" t="s">
-        <v>313</v>
+        <v>261</v>
       </c>
       <c r="AX6" s="2" t="s">
-        <v>314</v>
+        <v>262</v>
       </c>
       <c r="AY6" s="2" t="s">
-        <v>315</v>
+        <v>230</v>
       </c>
       <c r="AZ6" s="2" t="s">
-        <v>316</v>
+        <v>230</v>
       </c>
       <c r="BA6" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="BB6" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="BC6" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="BD6" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="BE6" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="BF6" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="BG6" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="BH6" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="BI6" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="BJ6" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="BK6" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="BL6" s="2" t="s">
-        <v>324</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>325</v>
+        <v>264</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>326</v>
+        <v>265</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>327</v>
+        <v>266</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>328</v>
+        <v>267</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>325</v>
+        <v>268</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>329</v>
+        <v>269</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>330</v>
+        <v>270</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>331</v>
+        <v>271</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>332</v>
+        <v>272</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>333</v>
+        <v>273</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>334</v>
+        <v>274</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>335</v>
+        <v>275</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>336</v>
+        <v>273</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>337</v>
+        <v>272</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>335</v>
+        <v>276</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>334</v>
+        <v>277</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>338</v>
+        <v>278</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>339</v>
+        <v>279</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>340</v>
+        <v>280</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>341</v>
+        <v>281</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>342</v>
+        <v>282</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>343</v>
+        <v>283</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>344</v>
+        <v>284</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>345</v>
+        <v>273</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>346</v>
+        <v>273</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>347</v>
+        <v>285</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>348</v>
+        <v>286</v>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>335</v>
+        <v>288</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>335</v>
+        <v>289</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>350</v>
+        <v>282</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>351</v>
+        <v>290</v>
       </c>
       <c r="AG7" s="2" t="s">
-        <v>352</v>
+        <v>291</v>
       </c>
       <c r="AH7" s="2" t="s">
-        <v>353</v>
+        <v>292</v>
       </c>
       <c r="AI7" s="2" t="s">
-        <v>354</v>
+        <v>293</v>
       </c>
       <c r="AJ7" s="2" t="s">
-        <v>355</v>
+        <v>272</v>
       </c>
       <c r="AK7" s="2" t="s">
-        <v>345</v>
+        <v>294</v>
       </c>
       <c r="AL7" s="2" t="s">
-        <v>356</v>
+        <v>293</v>
       </c>
       <c r="AM7" s="2" t="s">
-        <v>357</v>
+        <v>295</v>
       </c>
       <c r="AN7" s="2" t="s">
-        <v>358</v>
+        <v>296</v>
       </c>
       <c r="AO7" s="2" t="s">
-        <v>359</v>
+        <v>297</v>
       </c>
       <c r="AP7" s="2" t="s">
-        <v>360</v>
+        <v>298</v>
       </c>
       <c r="AQ7" s="2" t="s">
-        <v>334</v>
+        <v>299</v>
       </c>
       <c r="AR7" s="2" t="s">
-        <v>361</v>
+        <v>300</v>
       </c>
       <c r="AS7" s="2" t="s">
-        <v>360</v>
+        <v>274</v>
       </c>
       <c r="AT7" s="2" t="s">
-        <v>362</v>
+        <v>296</v>
       </c>
       <c r="AU7" s="2" t="s">
-        <v>363</v>
+        <v>301</v>
       </c>
       <c r="AV7" s="2" t="s">
-        <v>364</v>
+        <v>302</v>
       </c>
       <c r="AW7" s="2" t="s">
-        <v>365</v>
+        <v>303</v>
       </c>
       <c r="AX7" s="2" t="s">
-        <v>366</v>
+        <v>304</v>
       </c>
       <c r="AY7" s="2" t="s">
-        <v>367</v>
+        <v>272</v>
       </c>
       <c r="AZ7" s="2" t="s">
-        <v>368</v>
+        <v>272</v>
       </c>
       <c r="BA7" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="BB7" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="BC7" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="BD7" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="BE7" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="BF7" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="BG7" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="BH7" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="BI7" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="BJ7" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="BK7" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="BL7" s="2" t="s">
-        <v>376</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>